<commit_message>
Restructured code to accomodate manual edits to data ingested into the bot and future reise if structure of spreadsheet changes
Also added an example of the Credentials.py file
</commit_message>
<xml_diff>
--- a/data/minorsfixtures.xlsx
+++ b/data/minorsfixtures.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="26">
   <si>
     <t>Minors Fixtures</t>
   </si>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -471,6 +471,9 @@
       <alignment horizontal="right" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="17" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -3077,11 +3080,15 @@
         <f t="shared" ref="B46:B49" si="37">IF(A46="",,IFERROR(INDEX(Source!K:K,MATCH(A46,Source!I:I,0),0),"-"))</f>
         <v/>
       </c>
-      <c r="C46" s="14"/>
+      <c r="C46" s="14">
+        <v>6.0</v>
+      </c>
       <c r="D46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="14"/>
+      <c r="E46" s="14">
+        <v>4.0</v>
+      </c>
       <c r="F46" s="13" t="str">
         <f t="shared" ref="F46:F49" si="38">IF(G46="",,IFERROR(INDEX(Source!K:K,MATCH(G46,Source!I:I,0),0),"-"))</f>
         <v/>
@@ -3102,11 +3109,15 @@
         <f t="shared" ref="O46:O49" si="39">IF(L46="",,IFERROR(INDEX(Source!K:K,MATCH(L46,Source!I:I,0),0),"-"))</f>
         <v/>
       </c>
-      <c r="P46" s="14"/>
+      <c r="P46" s="14">
+        <v>13.0</v>
+      </c>
       <c r="Q46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R46" s="14"/>
+      <c r="R46" s="14">
+        <v>6.0</v>
+      </c>
       <c r="S46" s="13" t="str">
         <f t="shared" ref="S46:S49" si="40">IF(T46="",,IFERROR(INDEX(Source!K:K,MATCH(T46,Source!I:I,0),0),"-"))</f>
         <v/>
@@ -3122,11 +3133,15 @@
         <f t="shared" ref="W46:W49" si="41">IF(L46="",,IFERROR(INDEX(Source!K:K,MATCH(V46,Source!I:I,0),0),"-"))</f>
         <v/>
       </c>
-      <c r="X46" s="14"/>
+      <c r="X46" s="14">
+        <v>7.0</v>
+      </c>
       <c r="Y46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Z46" s="14"/>
+      <c r="Z46" s="14">
+        <v>1.0</v>
+      </c>
       <c r="AA46" s="13" t="str">
         <f t="shared" ref="AA46:AA49" si="42">IF(T46="",,IFERROR(INDEX(Source!K:K,MATCH(AB46,Source!I:I,0),0),"-"))</f>
         <v/>
@@ -3143,11 +3158,15 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="C47" s="14"/>
+      <c r="C47" s="14">
+        <v>4.0</v>
+      </c>
       <c r="D47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="14"/>
+      <c r="E47" s="14">
+        <v>7.0</v>
+      </c>
       <c r="F47" s="13" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -3168,11 +3187,15 @@
         <f t="shared" si="39"/>
         <v/>
       </c>
-      <c r="P47" s="14"/>
+      <c r="P47" s="14">
+        <v>15.0</v>
+      </c>
       <c r="Q47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R47" s="14"/>
+      <c r="R47" s="14">
+        <v>5.0</v>
+      </c>
       <c r="S47" s="13" t="str">
         <f t="shared" si="40"/>
         <v/>
@@ -3188,11 +3211,15 @@
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="X47" s="14"/>
+      <c r="X47" s="14">
+        <v>7.0</v>
+      </c>
       <c r="Y47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Z47" s="14"/>
+      <c r="Z47" s="14">
+        <v>7.0</v>
+      </c>
       <c r="AA47" s="13" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -3209,11 +3236,15 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="C48" s="14"/>
+      <c r="C48" s="14">
+        <v>5.0</v>
+      </c>
       <c r="D48" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="14"/>
+      <c r="E48" s="15">
+        <v>9.0</v>
+      </c>
       <c r="F48" s="13" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -3234,11 +3265,15 @@
         <f t="shared" si="39"/>
         <v/>
       </c>
-      <c r="P48" s="14"/>
+      <c r="P48" s="14">
+        <v>6.0</v>
+      </c>
       <c r="Q48" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R48" s="14"/>
+      <c r="R48" s="14">
+        <v>6.0</v>
+      </c>
       <c r="S48" s="13" t="str">
         <f t="shared" si="40"/>
         <v/>
@@ -3254,11 +3289,15 @@
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="X48" s="14"/>
+      <c r="X48" s="14">
+        <v>8.0</v>
+      </c>
       <c r="Y48" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Z48" s="14"/>
+      <c r="Z48" s="14">
+        <v>6.0</v>
+      </c>
       <c r="AA48" s="13" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -3275,11 +3314,15 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="C49" s="14"/>
+      <c r="C49" s="14">
+        <v>5.0</v>
+      </c>
       <c r="D49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="14"/>
+      <c r="E49" s="14">
+        <v>7.0</v>
+      </c>
       <c r="F49" s="13" t="str">
         <f t="shared" si="38"/>
         <v/>
@@ -3300,11 +3343,15 @@
         <f t="shared" si="39"/>
         <v/>
       </c>
-      <c r="P49" s="14"/>
+      <c r="P49" s="14">
+        <v>5.0</v>
+      </c>
       <c r="Q49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R49" s="14"/>
+      <c r="R49" s="14">
+        <v>3.0</v>
+      </c>
       <c r="S49" s="13" t="str">
         <f t="shared" si="40"/>
         <v/>
@@ -3320,11 +3367,15 @@
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="X49" s="14"/>
+      <c r="X49" s="14">
+        <v>3.0</v>
+      </c>
       <c r="Y49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Z49" s="14"/>
+      <c r="Z49" s="14">
+        <v>7.0</v>
+      </c>
       <c r="AA49" s="13" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -3422,7 +3473,9 @@
       <c r="AB52" s="10"/>
     </row>
     <row r="53" ht="18.75" customHeight="1">
-      <c r="A53" s="20"/>
+      <c r="A53" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="B53" s="13" t="str">
         <f t="shared" ref="B53:B54" si="43">IF(A53="",,IFERROR(INDEX(Source!K:K,MATCH(A53,Source!I:I,0),0),""))</f>
         <v/>
@@ -3436,7 +3489,9 @@
         <f t="shared" ref="F53:F54" si="44">IF(G53="",,IFERROR(INDEX(Source!K:K,MATCH(G53,Source!I:I,0),0),""))</f>
         <v/>
       </c>
-      <c r="G53" s="46"/>
+      <c r="G53" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="H53" s="60" t="s">
         <v>22</v>
       </c>
@@ -3445,7 +3500,9 @@
       <c r="L53" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="N53" s="20"/>
+      <c r="N53" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="O53" s="13" t="str">
         <f t="shared" ref="O53:O54" si="45">IF(N53="",,IFERROR(INDEX(Source!K:K,MATCH(N53,Source!I:I,0),0),""))</f>
         <v/>
@@ -3459,7 +3516,9 @@
         <f t="shared" ref="S53:S54" si="46">IF(T53="",,IFERROR(INDEX(Source!K:K,MATCH(T53,Source!I:I,0),0),""))</f>
         <v/>
       </c>
-      <c r="T53" s="46"/>
+      <c r="T53" s="40" t="s">
+        <v>11</v>
+      </c>
       <c r="U53" s="18"/>
       <c r="V53" s="18"/>
       <c r="W53" s="18"/>
@@ -3470,7 +3529,9 @@
       <c r="AB53" s="18"/>
     </row>
     <row r="54" ht="18.75" customHeight="1">
-      <c r="A54" s="52"/>
+      <c r="A54" s="52" t="s">
+        <v>6</v>
+      </c>
       <c r="B54" s="13" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -3484,7 +3545,9 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="G54" s="40"/>
+      <c r="G54" s="53" t="s">
+        <v>8</v>
+      </c>
       <c r="H54" s="60" t="s">
         <v>22</v>
       </c>
@@ -3493,7 +3556,9 @@
       <c r="L54" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="N54" s="52"/>
+      <c r="N54" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="O54" s="13" t="str">
         <f t="shared" si="45"/>
         <v/>
@@ -3507,9 +3572,11 @@
         <f t="shared" si="46"/>
         <v/>
       </c>
-      <c r="T54" s="40"/>
-      <c r="U54" s="18"/>
-      <c r="V54" s="18"/>
+      <c r="T54" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="U54" s="26"/>
+      <c r="V54" s="62"/>
       <c r="W54" s="18"/>
       <c r="X54" s="18"/>
       <c r="Y54" s="18"/>
@@ -3732,28 +3799,28 @@
       <c r="AB60" s="10"/>
     </row>
     <row r="61" ht="21.75" customHeight="1">
-      <c r="A61" s="62">
+      <c r="A61" s="63">
         <f>A56+7</f>
         <v>43990</v>
       </c>
-      <c r="B61" s="63"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="64" t="s">
+      <c r="B61" s="64"/>
+      <c r="G61" s="65"/>
+      <c r="H61" s="65"/>
+      <c r="I61" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="M61" s="64"/>
-      <c r="N61" s="64"/>
-      <c r="O61" s="63"/>
-      <c r="T61" s="64"/>
-      <c r="U61" s="64"/>
-      <c r="V61" s="64"/>
-      <c r="W61" s="64"/>
-      <c r="X61" s="64"/>
-      <c r="Y61" s="64"/>
-      <c r="Z61" s="64"/>
-      <c r="AA61" s="64"/>
-      <c r="AB61" s="64"/>
+      <c r="M61" s="65"/>
+      <c r="N61" s="65"/>
+      <c r="O61" s="64"/>
+      <c r="T61" s="65"/>
+      <c r="U61" s="65"/>
+      <c r="V61" s="65"/>
+      <c r="W61" s="65"/>
+      <c r="X61" s="65"/>
+      <c r="Y61" s="65"/>
+      <c r="Z61" s="65"/>
+      <c r="AA61" s="65"/>
+      <c r="AB61" s="65"/>
     </row>
     <row r="62" ht="7.5" customHeight="1">
       <c r="A62" s="9"/>
@@ -3786,26 +3853,26 @@
       <c r="AB62" s="10"/>
     </row>
     <row r="63" ht="21.75" customHeight="1">
-      <c r="A63" s="65"/>
-      <c r="B63" s="66" t="s">
+      <c r="A63" s="66"/>
+      <c r="B63" s="67" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="20"/>
-      <c r="H63" s="66" t="str">
+      <c r="H63" s="67" t="str">
         <f t="shared" ref="H63:H65" si="51">IF(G63="",,IFERROR(INDEX(Source!K:K,MATCH(G63,Source!I:I,0),0),""))</f>
         <v/>
       </c>
-      <c r="I63" s="67"/>
+      <c r="I63" s="68"/>
       <c r="J63" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L63" s="68"/>
-      <c r="M63" s="66" t="str">
+      <c r="L63" s="69"/>
+      <c r="M63" s="67" t="str">
         <f t="shared" ref="M63:M65" si="52">IF(N63="",,IFERROR(INDEX(Source!K:K,MATCH(N63,Source!I:I,0),0),""))</f>
         <v/>
       </c>
       <c r="N63" s="46"/>
-      <c r="O63" s="66" t="s">
+      <c r="O63" s="67" t="s">
         <v>22</v>
       </c>
       <c r="T63" s="18"/>
@@ -3819,26 +3886,26 @@
       <c r="AB63" s="18"/>
     </row>
     <row r="64" ht="21.75" customHeight="1">
-      <c r="A64" s="65"/>
-      <c r="B64" s="66" t="s">
+      <c r="A64" s="66"/>
+      <c r="B64" s="67" t="s">
         <v>22</v>
       </c>
       <c r="G64" s="33"/>
-      <c r="H64" s="66" t="str">
+      <c r="H64" s="67" t="str">
         <f t="shared" si="51"/>
         <v/>
       </c>
-      <c r="I64" s="67"/>
+      <c r="I64" s="68"/>
       <c r="J64" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L64" s="68"/>
-      <c r="M64" s="66" t="str">
+      <c r="L64" s="69"/>
+      <c r="M64" s="67" t="str">
         <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="N64" s="29"/>
-      <c r="O64" s="66" t="s">
+      <c r="O64" s="67" t="s">
         <v>22</v>
       </c>
       <c r="T64" s="18"/>
@@ -3852,26 +3919,26 @@
       <c r="AB64" s="18"/>
     </row>
     <row r="65" ht="21.75" customHeight="1">
-      <c r="A65" s="65"/>
-      <c r="B65" s="69" t="s">
+      <c r="A65" s="66"/>
+      <c r="B65" s="70" t="s">
         <v>22</v>
       </c>
       <c r="G65" s="52"/>
-      <c r="H65" s="66" t="str">
+      <c r="H65" s="67" t="str">
         <f t="shared" si="51"/>
         <v/>
       </c>
-      <c r="I65" s="70"/>
-      <c r="J65" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="L65" s="71"/>
-      <c r="M65" s="66" t="str">
+      <c r="I65" s="71"/>
+      <c r="J65" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="L65" s="72"/>
+      <c r="M65" s="67" t="str">
         <f t="shared" si="52"/>
         <v/>
       </c>
-      <c r="N65" s="72"/>
-      <c r="O65" s="69" t="s">
+      <c r="N65" s="73"/>
+      <c r="O65" s="70" t="s">
         <v>22</v>
       </c>
       <c r="T65" s="18"/>
@@ -3885,34 +3952,34 @@
       <c r="AB65" s="18"/>
     </row>
     <row r="66" ht="7.5" customHeight="1">
-      <c r="A66" s="73"/>
-      <c r="B66" s="73"/>
-      <c r="C66" s="74"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="75"/>
-      <c r="J66" s="75"/>
-      <c r="K66" s="75"/>
-      <c r="L66" s="75"/>
-      <c r="M66" s="75"/>
-      <c r="N66" s="75"/>
-      <c r="O66" s="75"/>
-      <c r="P66" s="75"/>
-      <c r="Q66" s="75"/>
-      <c r="R66" s="75"/>
-      <c r="S66" s="75"/>
-      <c r="T66" s="75"/>
-      <c r="U66" s="75"/>
-      <c r="V66" s="75"/>
-      <c r="W66" s="75"/>
-      <c r="X66" s="75"/>
-      <c r="Y66" s="75"/>
-      <c r="Z66" s="75"/>
-      <c r="AA66" s="75"/>
-      <c r="AB66" s="75"/>
+      <c r="A66" s="74"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="76"/>
+      <c r="M66" s="76"/>
+      <c r="N66" s="76"/>
+      <c r="O66" s="76"/>
+      <c r="P66" s="76"/>
+      <c r="Q66" s="76"/>
+      <c r="R66" s="76"/>
+      <c r="S66" s="76"/>
+      <c r="T66" s="76"/>
+      <c r="U66" s="76"/>
+      <c r="V66" s="76"/>
+      <c r="W66" s="76"/>
+      <c r="X66" s="76"/>
+      <c r="Y66" s="76"/>
+      <c r="Z66" s="76"/>
+      <c r="AA66" s="76"/>
+      <c r="AB66" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="97">

</xml_diff>